<commit_message>
Bugfixes and Thermocycler Improvements
</commit_message>
<xml_diff>
--- a/volume_calculator.xlsx
+++ b/volume_calculator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megam\OneDrive\Desktop\MoCloScript\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\opentrons\Desktop\MilesV\MoCloScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3D5E9B5-AAE6-44B2-B859-6EAAD6447C5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68876561-DBE2-465E-BF81-36AC0FD9FB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{CF1C542D-9FFD-418A-91F0-D25BE1CEE975}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CF1C542D-9FFD-418A-91F0-D25BE1CEE975}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculator" sheetId="1" r:id="rId1"/>
@@ -500,22 +500,22 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.19921875" customWidth="1"/>
-    <col min="2" max="2" width="20.265625" customWidth="1"/>
-    <col min="3" max="3" width="11.86328125" customWidth="1"/>
-    <col min="4" max="4" width="16.19921875" customWidth="1"/>
-    <col min="5" max="5" width="15.06640625" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="24.59765625" customWidth="1"/>
-    <col min="9" max="9" width="26.19921875" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,7 +544,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -576,7 +576,7 @@
         <v>3.3434375000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -608,7 +608,7 @@
         <v>2.5685833333333337</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -640,7 +640,7 @@
         <v>2.8616250000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -672,7 +672,7 @@
         <v>1.07406</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -704,7 +704,7 @@
         <v>1.2012812500000001</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -736,36 +736,36 @@
         <v>20.163</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="3">
-        <v>100</v>
+        <v>308</v>
       </c>
       <c r="C8" s="3">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D8" s="3">
-        <v>2247</v>
+        <v>1646</v>
       </c>
       <c r="E8" s="3">
-        <v>2846</v>
+        <v>2676</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" si="0"/>
-        <v>73.027500000000003</v>
+        <v>26.747499999999999</v>
       </c>
       <c r="G8" s="4">
         <f t="shared" si="1"/>
-        <v>92.495000000000005</v>
+        <v>43.484999999999999</v>
       </c>
       <c r="H8" s="3">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I8" s="4">
         <f t="shared" si="2"/>
-        <v>1.8499000000000001</v>
+        <v>0.98829545454545453</v>
       </c>
     </row>
   </sheetData>

</xml_diff>